<commit_message>
update 3 tests: added data when don't in file
</commit_message>
<xml_diff>
--- a/src/tests/java/auth/dev/net/data_files/text_registration_page_data.xlsx
+++ b/src/tests/java/auth/dev/net/data_files/text_registration_page_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="textUA" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="103">
   <si>
     <t>testName</t>
   </si>
@@ -59,24 +59,9 @@
     <t>Як вас звати?</t>
   </si>
   <si>
-    <t>Ім'я</t>
-  </si>
-  <si>
-    <t>Прізвище</t>
-  </si>
-  <si>
     <t>Дата народження</t>
   </si>
   <si>
-    <t>число</t>
-  </si>
-  <si>
-    <t>місяць</t>
-  </si>
-  <si>
-    <t>рік</t>
-  </si>
-  <si>
     <t>Чоловік</t>
   </si>
   <si>
@@ -98,9 +83,6 @@
     <t>Поштову скриньку необхідно активувати</t>
   </si>
   <si>
-    <t>На вказаний номер мобільного телефону буде відправлено SMS з кодом активації</t>
-  </si>
-  <si>
     <t>ОТРИМАТИ КОД</t>
   </si>
   <si>
@@ -209,27 +191,9 @@
     <t>//form/section[1]/div/span</t>
   </si>
   <si>
-    <t>//section[3]/section[1]/div/div[1]/input</t>
-  </si>
-  <si>
-    <t>//section[3]/section[1]/div/div[2]/input</t>
-  </si>
-  <si>
-    <t>//section[3]/section[2]/div/div[1]/input</t>
-  </si>
-  <si>
-    <t>//section[3]/section[2]/div/div[2]/input</t>
-  </si>
-  <si>
-    <t>//section[3]/section[2]/div/div[3]/input</t>
-  </si>
-  <si>
     <t>//section[6]/div/div/div/span</t>
   </si>
   <si>
-    <t>//section[7]/button/span[1]</t>
-  </si>
-  <si>
     <t>//div[1]/div/div[2]</t>
   </si>
   <si>
@@ -239,9 +203,6 @@
     <t>ЦІЛОДОБОВА ПІДТРИМКА</t>
   </si>
   <si>
-    <t>textUkrNO</t>
-  </si>
-  <si>
     <t>//button[text()]</t>
   </si>
   <si>
@@ -251,9 +212,6 @@
     <t>textRu</t>
   </si>
   <si>
-    <t>textRuNO</t>
-  </si>
-  <si>
     <t>Регистрация почтового ящика</t>
   </si>
   <si>
@@ -272,21 +230,9 @@
     <t>Как вас зовут?</t>
   </si>
   <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Фамилия</t>
-  </si>
-  <si>
     <t>Дата рождения</t>
   </si>
   <si>
-    <t>месяц</t>
-  </si>
-  <si>
-    <t>год</t>
-  </si>
-  <si>
     <t>Мужчина</t>
   </si>
   <si>
@@ -303,9 +249,6 @@
   </si>
   <si>
     <t>Почтовый ящик необходимо активировать</t>
-  </si>
-  <si>
-    <t>На указанный номер мобильного телефона будет отправлено SMS с кодом активации</t>
   </si>
   <si>
     <t>ПОЛУЧИТЬ КОД</t>
@@ -327,9 +270,6 @@
 с Соглашением о конфиденциальности и принимаю его условия.</t>
   </si>
   <si>
-    <t>Create mailbox</t>
-  </si>
-  <si>
     <t>Create Your @UKR.NET Mailbox</t>
   </si>
   <si>
@@ -351,24 +291,9 @@
     <t>Your name</t>
   </si>
   <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
     <t>Birthdate</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -384,12 +309,6 @@
     <t>You should activate your mailbox</t>
   </si>
   <si>
-    <t>A message with an activation code will be sent to the number provided here</t>
-  </si>
-  <si>
-    <t>GET THE VERIFICATION CODE</t>
-  </si>
-  <si>
     <t>Start importing my mail from other email providers</t>
   </si>
   <si>
@@ -399,9 +318,6 @@
     <t>textEn</t>
   </si>
   <si>
-    <t>textEnNO</t>
-  </si>
-  <si>
     <t>Sender’s name</t>
   </si>
   <si>
@@ -409,6 +325,12 @@
   </si>
   <si>
     <t>I herein consent to my personal data processing in accordance with Privacy Policy which I have read and agreed to.</t>
+  </si>
+  <si>
+    <t>GET ACTIVATION CODE</t>
+  </si>
+  <si>
+    <t>Create your @UKR.NET mailbox</t>
   </si>
 </sst>
 </file>
@@ -771,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AME36"/>
+  <dimension ref="A1:AME30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,400 +712,334 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
@@ -1192,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,400 +1066,334 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>62</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>62</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>100</v>
+        <v>62</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1611,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,400 +1419,334 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>97</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>128</v>
+        <v>97</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>